<commit_message>
accumlated: footerNotes, invNote, ...
</commit_message>
<xml_diff>
--- a/printer/templates/receipt.xlsx
+++ b/printer/templates/receipt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafat\Desktop\TemplatePrinting\printer\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafat\source\- back\template-printing-api\printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Configuration Sheet</t>
   </si>
@@ -133,19 +133,22 @@
     <t>{{InvoiceNo}}</t>
   </si>
   <si>
-    <t>{{note1}}</t>
-  </si>
-  <si>
-    <t>{{note2}}</t>
-  </si>
-  <si>
-    <t>{{note3}}</t>
-  </si>
-  <si>
     <t>{{DeliveryNameTitle}}</t>
   </si>
   <si>
     <t>{{DeliveryName}}</t>
+  </si>
+  <si>
+    <t>{{Note}}</t>
+  </si>
+  <si>
+    <t>{{FooterNote2}}</t>
+  </si>
+  <si>
+    <t>{{FooterNote1}}</t>
+  </si>
+  <si>
+    <t>{{FooterNote3}}</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
@@ -558,6 +561,9 @@
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,10 +573,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -596,24 +599,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1486,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:G16"/>
+      <selection activeCell="A27" sqref="A27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1506,12 +1491,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="6"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1526,35 +1511,35 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="6"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="6"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
       <c r="E5" s="6"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1571,15 +1556,15 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="3.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1593,46 +1578,46 @@
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33" t="s">
+      <c r="E9" s="34"/>
+      <c r="F9" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="33"/>
+      <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="52" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52" t="s">
+      <c r="E10" s="46"/>
+      <c r="F10" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="52"/>
+      <c r="G10" s="46"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
+      <c r="A11" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
       <c r="G11" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="2.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1682,13 +1667,13 @@
       <c r="B16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="56"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="50"/>
     </row>
     <row r="17" spans="1:10" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
@@ -1703,14 +1688,14 @@
       <c r="A18" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
     </row>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
@@ -1731,25 +1716,25 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="47"/>
+      <c r="A21" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
       <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1762,7 +1747,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="37" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
@@ -1784,8 +1769,8 @@
     </row>
     <row r="26" spans="1:10" ht="8.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
-        <v>37</v>
+      <c r="A27" s="36" t="s">
+        <v>40</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
@@ -1794,8 +1779,28 @@
       <c r="F27" s="36"/>
       <c r="G27" s="36"/>
     </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A24:G25"/>
     <mergeCell ref="A13:F13"/>
@@ -1806,14 +1811,6 @@
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="120" scale="69" fitToHeight="0" orientation="portrait" horizontalDpi="120" verticalDpi="144" r:id="rId1"/>

</xml_diff>

<commit_message>
add visa & visa percent properties
</commit_message>
<xml_diff>
--- a/printer/templates/receipt.xlsx
+++ b/printer/templates/receipt.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafat\source\- back\template-printing-api\printer\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafat\source\__\template-printing-api\printer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="25935" windowHeight="20985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Configuration Sheet</t>
   </si>
@@ -167,6 +167,18 @@
   </si>
   <si>
     <t>printing-time</t>
+  </si>
+  <si>
+    <t>{{Visa}}</t>
+  </si>
+  <si>
+    <t>visa-per</t>
+  </si>
+  <si>
+    <t>{{VisaPer}}</t>
+  </si>
+  <si>
+    <t>{{VisaPerTitle}}</t>
   </si>
 </sst>
 </file>
@@ -667,6 +679,12 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,6 +700,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
     </xf>
@@ -732,15 +753,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1676,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:G33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="160" zoomScaleNormal="145" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1694,12 +1706,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="6"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1714,10 +1726,10 @@
       <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="34"/>
       <c r="F3" s="36" t="s">
         <v>29</v>
@@ -1725,24 +1737,24 @@
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="6"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="6"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1759,27 +1771,27 @@
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
       <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" ht="3.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1803,17 +1815,17 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="3.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1827,34 +1839,34 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="22.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="39" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39" t="s">
+      <c r="E13" s="41"/>
+      <c r="F13" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="39"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="55" t="s">
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="54" t="s">
+      <c r="E14" s="58"/>
+      <c r="F14" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="54"/>
+      <c r="G14" s="57"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
@@ -1875,14 +1887,14 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="17.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
       <c r="G17" s="37" t="s">
         <v>25</v>
       </c>
@@ -1912,13 +1924,13 @@
       <c r="B20" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="59"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
     </row>
     <row r="21" spans="1:10" ht="3.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
@@ -1933,14 +1945,14 @@
       <c r="A22" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="53"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="56"/>
     </row>
     <row r="23" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
@@ -1961,25 +1973,25 @@
       <c r="J24" s="10"/>
     </row>
     <row r="25" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="45" t="s">
+      <c r="A25" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="50"/>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="53"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="1:10" ht="3.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,76 +2003,92 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
       <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="61" t="s">
+      <c r="A33" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="63" spans="5:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="E63" s="30"/>

</xml_diff>